<commit_message>
chore: a couple updates from design review
- add DXF layer for board outline footprint
- remove copper restrict from under camera mounts
- move FFC x-0.4mm to align with camera board(was off previously)
- add parts for I2C0 ESD circuit to BOM
</commit_message>
<xml_diff>
--- a/oresat-camera-hardware/star-tracker-card/star-tracker-card-digikey-bom.xlsx
+++ b/oresat-camera-hardware/star-tracker-card/star-tracker-card-digikey-bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliver.rew/oresat/oresat-star-tracker/oresat-camera-hardware/star-tracker-card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F854F6-1F06-CD43-A40A-EDA442288D7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53AE7B0-AE54-B143-A157-ABE17198A5CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="19020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -676,9 +676,6 @@
     <t>445-5667-1-ND</t>
   </si>
   <si>
-    <t>C4,11,16,17,18,20,21,24,25,26,28,31,39,40</t>
-  </si>
-  <si>
     <t>$0.79</t>
   </si>
   <si>
@@ -814,9 +811,6 @@
     <t>P100HCT-ND</t>
   </si>
   <si>
-    <t>R41, R48, R71</t>
-  </si>
-  <si>
     <t>RES SMD 100 OHM 1% 1/10W 0603</t>
   </si>
   <si>
@@ -872,6 +866,12 @@
   </si>
   <si>
     <t>R6,7,11,12,14-16,19-22,28,32,34,35,39,43,46,52,64,72</t>
+  </si>
+  <si>
+    <t>R41, R48, R71, R73, R74, R75</t>
+  </si>
+  <si>
+    <t>C4,11,16,17,18,20,21,24,25,26,28,31,39,40,41</t>
   </si>
 </sst>
 </file>
@@ -1228,11 +1228,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
@@ -1251,7 +1251,7 @@
     <col min="15" max="16" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>101</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>125</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>137</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>149</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>155</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>22</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I24">
         <v>1.02</v>
@@ -2451,7 +2451,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>162</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>168</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>175</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>179</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>186</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>191</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>197</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>202</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>207</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>212</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>216</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>217</v>
       </c>
       <c r="D35" t="s">
-        <v>218</v>
+        <v>283</v>
       </c>
       <c r="E35" t="s">
         <v>20</v>
@@ -2974,13 +2974,13 @@
         <v>22</v>
       </c>
       <c r="H35">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I35">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="J35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K35">
         <v>1804980</v>
@@ -2989,7 +2989,7 @@
         <v>43</v>
       </c>
       <c r="M35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N35" t="s">
         <v>26</v>
@@ -3001,18 +3001,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>220</v>
+      </c>
+      <c r="B36" t="s">
         <v>221</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>222</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>223</v>
-      </c>
-      <c r="D36" t="s">
-        <v>224</v>
       </c>
       <c r="E36" t="s">
         <v>20</v>
@@ -3030,7 +3030,7 @@
         <v>0.35</v>
       </c>
       <c r="J36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K36">
         <v>15088</v>
@@ -3039,7 +3039,7 @@
         <v>43</v>
       </c>
       <c r="M36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N36" t="s">
         <v>26</v>
@@ -3051,18 +3051,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>226</v>
+      </c>
+      <c r="B37" t="s">
+        <v>221</v>
+      </c>
+      <c r="C37" t="s">
         <v>227</v>
       </c>
-      <c r="B37" t="s">
-        <v>222</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>228</v>
-      </c>
-      <c r="D37" t="s">
-        <v>229</v>
       </c>
       <c r="E37" t="s">
         <v>20</v>
@@ -3080,7 +3080,7 @@
         <v>0.35</v>
       </c>
       <c r="J37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K37">
         <v>7514</v>
@@ -3089,7 +3089,7 @@
         <v>43</v>
       </c>
       <c r="M37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N37" t="s">
         <v>26</v>
@@ -3101,18 +3101,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>230</v>
+      </c>
+      <c r="B38" t="s">
+        <v>221</v>
+      </c>
+      <c r="C38" t="s">
         <v>231</v>
       </c>
-      <c r="B38" t="s">
-        <v>222</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>232</v>
-      </c>
-      <c r="D38" t="s">
-        <v>233</v>
       </c>
       <c r="E38" t="s">
         <v>20</v>
@@ -3139,7 +3139,7 @@
         <v>43</v>
       </c>
       <c r="M38" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N38" t="s">
         <v>26</v>
@@ -3151,18 +3151,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B39" t="s">
         <v>169</v>
       </c>
       <c r="C39" t="s">
+        <v>234</v>
+      </c>
+      <c r="D39" t="s">
         <v>235</v>
-      </c>
-      <c r="D39" t="s">
-        <v>236</v>
       </c>
       <c r="E39" t="s">
         <v>20</v>
@@ -3180,7 +3180,7 @@
         <v>0.1</v>
       </c>
       <c r="J39" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K39">
         <v>489828</v>
@@ -3189,7 +3189,7 @@
         <v>112</v>
       </c>
       <c r="M39" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N39" t="s">
         <v>26</v>
@@ -3201,18 +3201,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B40" t="s">
         <v>169</v>
       </c>
       <c r="C40" t="s">
+        <v>239</v>
+      </c>
+      <c r="D40" t="s">
         <v>240</v>
-      </c>
-      <c r="D40" t="s">
-        <v>241</v>
       </c>
       <c r="E40" t="s">
         <v>20</v>
@@ -3230,7 +3230,7 @@
         <v>0.1</v>
       </c>
       <c r="J40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K40">
         <v>65782</v>
@@ -3239,7 +3239,7 @@
         <v>112</v>
       </c>
       <c r="M40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N40" t="s">
         <v>26</v>
@@ -3251,18 +3251,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B41" t="s">
         <v>169</v>
       </c>
       <c r="C41" t="s">
+        <v>244</v>
+      </c>
+      <c r="D41" t="s">
         <v>245</v>
-      </c>
-      <c r="D41" t="s">
-        <v>246</v>
       </c>
       <c r="E41" t="s">
         <v>20</v>
@@ -3289,7 +3289,7 @@
         <v>112</v>
       </c>
       <c r="M41" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N41" t="s">
         <v>26</v>
@@ -3301,18 +3301,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B42" t="s">
         <v>169</v>
       </c>
       <c r="C42" t="s">
+        <v>248</v>
+      </c>
+      <c r="D42" t="s">
         <v>249</v>
-      </c>
-      <c r="D42" t="s">
-        <v>250</v>
       </c>
       <c r="E42" t="s">
         <v>20</v>
@@ -3330,7 +3330,7 @@
         <v>0.1</v>
       </c>
       <c r="J42" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K42">
         <v>298436</v>
@@ -3339,7 +3339,7 @@
         <v>112</v>
       </c>
       <c r="M42" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N42" t="s">
         <v>26</v>
@@ -3351,18 +3351,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B43" t="s">
         <v>169</v>
       </c>
       <c r="C43" t="s">
+        <v>253</v>
+      </c>
+      <c r="D43" t="s">
         <v>254</v>
-      </c>
-      <c r="D43" t="s">
-        <v>255</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
@@ -3380,7 +3380,7 @@
         <v>0.1</v>
       </c>
       <c r="J43" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K43">
         <v>118618</v>
@@ -3389,7 +3389,7 @@
         <v>112</v>
       </c>
       <c r="M43" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N43" t="s">
         <v>26</v>
@@ -3401,18 +3401,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B44" t="s">
         <v>169</v>
       </c>
       <c r="C44" t="s">
+        <v>257</v>
+      </c>
+      <c r="D44" t="s">
         <v>258</v>
-      </c>
-      <c r="D44" t="s">
-        <v>259</v>
       </c>
       <c r="E44" t="s">
         <v>20</v>
@@ -3430,7 +3430,7 @@
         <v>0.1</v>
       </c>
       <c r="J44" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K44">
         <v>606430</v>
@@ -3439,7 +3439,7 @@
         <v>112</v>
       </c>
       <c r="M44" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N44" t="s">
         <v>26</v>
@@ -3451,18 +3451,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B45" t="s">
         <v>169</v>
       </c>
       <c r="C45" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D45" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="E45" t="s">
         <v>20</v>
@@ -3474,13 +3474,13 @@
         <v>22</v>
       </c>
       <c r="H45">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I45">
         <v>0.1</v>
       </c>
       <c r="J45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K45">
         <v>746294</v>
@@ -3489,7 +3489,7 @@
         <v>112</v>
       </c>
       <c r="M45" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="N45" t="s">
         <v>26</v>
@@ -3501,18 +3501,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B46" t="s">
         <v>169</v>
       </c>
       <c r="C46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D46" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E46" t="s">
         <v>20</v>
@@ -3530,7 +3530,7 @@
         <v>0.1</v>
       </c>
       <c r="J46" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K46">
         <v>12317582</v>
@@ -3539,7 +3539,7 @@
         <v>112</v>
       </c>
       <c r="M46" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="N46" t="s">
         <v>26</v>
@@ -3551,18 +3551,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B47" t="s">
         <v>169</v>
       </c>
       <c r="C47" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D47" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E47" t="s">
         <v>20</v>
@@ -3580,7 +3580,7 @@
         <v>0.1</v>
       </c>
       <c r="J47" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K47">
         <v>120542</v>
@@ -3589,7 +3589,7 @@
         <v>112</v>
       </c>
       <c r="M47" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="N47" t="s">
         <v>26</v>
@@ -3601,18 +3601,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B48" t="s">
         <v>169</v>
       </c>
       <c r="C48" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D48" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E48" t="s">
         <v>20</v>
@@ -3639,7 +3639,7 @@
         <v>112</v>
       </c>
       <c r="M48" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="N48" t="s">
         <v>26</v>
@@ -3651,18 +3651,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>275</v>
+      </c>
+      <c r="B49" t="s">
+        <v>276</v>
+      </c>
+      <c r="C49" t="s">
         <v>277</v>
       </c>
-      <c r="B49" t="s">
+      <c r="D49" t="s">
         <v>278</v>
-      </c>
-      <c r="C49" t="s">
-        <v>279</v>
-      </c>
-      <c r="D49" t="s">
-        <v>280</v>
       </c>
       <c r="E49" t="s">
         <v>20</v>
@@ -3680,7 +3680,7 @@
         <v>0.7</v>
       </c>
       <c r="J49" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K49">
         <v>24887</v>
@@ -3689,7 +3689,7 @@
         <v>24</v>
       </c>
       <c r="M49" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="N49" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
updated BOM with extra caps
</commit_message>
<xml_diff>
--- a/oresat-camera-hardware/star-tracker-card/star-tracker-card-digikey-bom.xlsx
+++ b/oresat-camera-hardware/star-tracker-card/star-tracker-card-digikey-bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliver.rew/oresat/oresat-star-tracker/oresat-camera-hardware/star-tracker-card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53AE7B0-AE54-B143-A157-ABE17198A5CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F733D39-7795-0E41-A439-A43EA5DDF09B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="19020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32060" windowHeight="19020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="246">
   <si>
     <t>Manufacturer Part Number</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Active</t>
   </si>
   <si>
-    <t>$43.73</t>
-  </si>
-  <si>
     <t>10 Weeks</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>Cut Tape (CT)</t>
   </si>
   <si>
-    <t>$0.84</t>
-  </si>
-  <si>
     <t>4 Weeks</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
     <t>U6</t>
   </si>
   <si>
-    <t>$6.44</t>
-  </si>
-  <si>
     <t>12 Weeks</t>
   </si>
   <si>
@@ -166,9 +157,6 @@
     <t>U5</t>
   </si>
   <si>
-    <t>$3.10</t>
-  </si>
-  <si>
     <t>IC TRNSLTR BIDIRECTIONAL 24TSSOP</t>
   </si>
   <si>
@@ -181,9 +169,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>$0.66</t>
-  </si>
-  <si>
     <t>IC PWR SWITCH N-CHAN 1:1 SOT23-5</t>
   </si>
   <si>
@@ -196,9 +181,6 @@
     <t>U9</t>
   </si>
   <si>
-    <t>$0.83</t>
-  </si>
-  <si>
     <t>6 Weeks</t>
   </si>
   <si>
@@ -214,9 +196,6 @@
     <t>U10</t>
   </si>
   <si>
-    <t>$0.98</t>
-  </si>
-  <si>
     <t>IC VREF SHUNT 18V 0.5% SOT23-3</t>
   </si>
   <si>
@@ -229,9 +208,6 @@
     <t>U15</t>
   </si>
   <si>
-    <t>$2.33</t>
-  </si>
-  <si>
     <t>8 Weeks</t>
   </si>
   <si>
@@ -247,9 +223,6 @@
     <t>U8</t>
   </si>
   <si>
-    <t>$0.35</t>
-  </si>
-  <si>
     <t>IC REG LINEAR 2.8V 200MA SOT23-5</t>
   </si>
   <si>
@@ -274,9 +247,6 @@
     <t>U4</t>
   </si>
   <si>
-    <t>$0.29</t>
-  </si>
-  <si>
     <t>IC BUF NON-INVERT 5.5V SC70-5</t>
   </si>
   <si>
@@ -292,9 +262,6 @@
     <t>FB1, FB2</t>
   </si>
   <si>
-    <t>$0.24</t>
-  </si>
-  <si>
     <t>7 Weeks</t>
   </si>
   <si>
@@ -313,9 +280,6 @@
     <t>Y2</t>
   </si>
   <si>
-    <t>$0.71</t>
-  </si>
-  <si>
     <t>29 Weeks</t>
   </si>
   <si>
@@ -337,9 +301,6 @@
     <t>U12, U13</t>
   </si>
   <si>
-    <t>$1.12</t>
-  </si>
-  <si>
     <t>IC COMP SNGL W/REF SC70-5</t>
   </si>
   <si>
@@ -355,9 +316,6 @@
     <t>J1</t>
   </si>
   <si>
-    <t>$0.95</t>
-  </si>
-  <si>
     <t>17 Weeks</t>
   </si>
   <si>
@@ -373,9 +331,6 @@
     <t>J101</t>
   </si>
   <si>
-    <t>$1.58</t>
-  </si>
-  <si>
     <t>CONN FPC BOTTOM 36POS 0.50MM R/A</t>
   </si>
   <si>
@@ -391,9 +346,6 @@
     <t>J100</t>
   </si>
   <si>
-    <t>$2.52</t>
-  </si>
-  <si>
     <t>CONN MICRO SD CARD PUSH-PUSH R/A</t>
   </si>
   <si>
@@ -409,9 +361,6 @@
     <t>Q3</t>
   </si>
   <si>
-    <t>$0.40</t>
-  </si>
-  <si>
     <t>16 Weeks</t>
   </si>
   <si>
@@ -427,9 +376,6 @@
     <t>Q5, Q6</t>
   </si>
   <si>
-    <t>$1.00</t>
-  </si>
-  <si>
     <t>MOSFET P CH 30V 4.5A TSOT26</t>
   </si>
   <si>
@@ -448,9 +394,6 @@
     <t>Tube</t>
   </si>
   <si>
-    <t>$3.58</t>
-  </si>
-  <si>
     <t>IC CURRENT MONITOR 1.5% 16TQFN</t>
   </si>
   <si>
@@ -463,9 +406,6 @@
     <t>U16</t>
   </si>
   <si>
-    <t>$3.76</t>
-  </si>
-  <si>
     <t>IC I/O EXPANDER I2C 8B 16TQFN</t>
   </si>
   <si>
@@ -478,9 +418,6 @@
     <t>Q1</t>
   </si>
   <si>
-    <t>$0.13</t>
-  </si>
-  <si>
     <t>15 Weeks</t>
   </si>
   <si>
@@ -499,9 +436,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>$1.02</t>
-  </si>
-  <si>
     <t>28 Weeks</t>
   </si>
   <si>
@@ -520,9 +454,6 @@
     <t>U3</t>
   </si>
   <si>
-    <t>$13.59</t>
-  </si>
-  <si>
     <t>16GB V5.1 I TEMP EMMC</t>
   </si>
   <si>
@@ -538,9 +469,6 @@
     <t>R8, R9, R10</t>
   </si>
   <si>
-    <t>$1.98</t>
-  </si>
-  <si>
     <t>13 Weeks</t>
   </si>
   <si>
@@ -571,9 +499,6 @@
     <t>L1</t>
   </si>
   <si>
-    <t>$1.65</t>
-  </si>
-  <si>
     <t>9 Weeks</t>
   </si>
   <si>
@@ -589,9 +514,6 @@
     <t>Y1</t>
   </si>
   <si>
-    <t>$0.86</t>
-  </si>
-  <si>
     <t>CRYSTAL 24MHZ 12PF SMD</t>
   </si>
   <si>
@@ -607,9 +529,6 @@
     <t>C1, C2, C7, C8, C38</t>
   </si>
   <si>
-    <t>$2.35</t>
-  </si>
-  <si>
     <t>CAP CER 10UF 16V X7S 0805</t>
   </si>
   <si>
@@ -622,9 +541,6 @@
     <t>C13, C14, C15, C36</t>
   </si>
   <si>
-    <t>$4.40</t>
-  </si>
-  <si>
     <t>CAP CER 22UF 16V X7R 1210</t>
   </si>
   <si>
@@ -637,9 +553,6 @@
     <t>C19, C22, C29, C30</t>
   </si>
   <si>
-    <t>$0.72</t>
-  </si>
-  <si>
     <t>CAP CER 18PF 50V C0G 0603</t>
   </si>
   <si>
@@ -652,9 +565,6 @@
     <t>C3, C5, C6, C9, C10, C12, C23, C27, C34, C37</t>
   </si>
   <si>
-    <t>$0.91</t>
-  </si>
-  <si>
     <t>CAP CER 1UF 16V X7R 0603</t>
   </si>
   <si>
@@ -676,9 +586,6 @@
     <t>445-5667-1-ND</t>
   </si>
   <si>
-    <t>$0.79</t>
-  </si>
-  <si>
     <t>CAP CER 0.1UF 25V X7R 0603</t>
   </si>
   <si>
@@ -694,9 +601,6 @@
     <t>D1, D7, D8</t>
   </si>
   <si>
-    <t>$1.05</t>
-  </si>
-  <si>
     <t>WL-SMCW SMT MONO-COLOR CHIP LED</t>
   </si>
   <si>
@@ -709,9 +613,6 @@
     <t>D2, D3, D4, D5</t>
   </si>
   <si>
-    <t>$1.40</t>
-  </si>
-  <si>
     <t>150060AS75020</t>
   </si>
   <si>
@@ -730,9 +631,6 @@
     <t>R1, R2, R3, R4, R5</t>
   </si>
   <si>
-    <t>$0.50</t>
-  </si>
-  <si>
     <t>RES SMD 1K OHM 1% 1/10W 0603</t>
   </si>
   <si>
@@ -745,9 +643,6 @@
     <t>R13, R36, R44</t>
   </si>
   <si>
-    <t>$0.30</t>
-  </si>
-  <si>
     <t>RES SMD 1M OHM 1% 1/10W 0603</t>
   </si>
   <si>
@@ -772,9 +667,6 @@
     <t>R23</t>
   </si>
   <si>
-    <t>$0.10</t>
-  </si>
-  <si>
     <t>RES SMD 499 OHM 1% 1/10W 0603</t>
   </si>
   <si>
@@ -799,9 +691,6 @@
     <t>R37, R45</t>
   </si>
   <si>
-    <t>$0.20</t>
-  </si>
-  <si>
     <t>RES SMD 330K OHM 1% 1/10W 0603</t>
   </si>
   <si>
@@ -857,9 +746,6 @@
   </si>
   <si>
     <t>R63</t>
-  </si>
-  <si>
-    <t>$0.70</t>
   </si>
   <si>
     <t>RES 0.1 OHM 1% 1/2W 1206</t>
@@ -1228,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1329,46 +1215,43 @@
       <c r="I2">
         <v>43.73</v>
       </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
       <c r="K2">
         <v>887</v>
       </c>
       <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" t="s">
         <v>27</v>
-      </c>
-      <c r="P2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
       <c r="E3" t="s">
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
@@ -1379,46 +1262,43 @@
       <c r="I3">
         <v>0.42</v>
       </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
       <c r="K3">
         <v>45504</v>
       </c>
       <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" t="s">
         <v>35</v>
-      </c>
-      <c r="M3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -1429,46 +1309,43 @@
       <c r="I4">
         <v>6.44</v>
       </c>
-      <c r="J4" t="s">
-        <v>42</v>
-      </c>
       <c r="K4">
         <v>2245</v>
       </c>
       <c r="L4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
         <v>22</v>
@@ -1479,46 +1356,43 @@
       <c r="I5">
         <v>3.1</v>
       </c>
-      <c r="J5" t="s">
-        <v>48</v>
-      </c>
       <c r="K5">
         <v>114</v>
       </c>
       <c r="L5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="N5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
         <v>22</v>
@@ -1529,46 +1403,43 @@
       <c r="I6">
         <v>0.66</v>
       </c>
-      <c r="J6" t="s">
-        <v>53</v>
-      </c>
       <c r="K6">
         <v>26392</v>
       </c>
       <c r="L6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
         <v>22</v>
@@ -1579,46 +1450,43 @@
       <c r="I7">
         <v>0.83</v>
       </c>
-      <c r="J7" t="s">
-        <v>58</v>
-      </c>
       <c r="K7">
         <v>11878</v>
       </c>
       <c r="L7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="M7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="N7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
         <v>22</v>
@@ -1629,46 +1497,43 @@
       <c r="I8">
         <v>0.98</v>
       </c>
-      <c r="J8" t="s">
-        <v>64</v>
-      </c>
       <c r="K8">
         <v>4022</v>
       </c>
       <c r="L8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="M8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="N8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
         <v>22</v>
@@ -1679,46 +1544,43 @@
       <c r="I9">
         <v>2.33</v>
       </c>
-      <c r="J9" t="s">
-        <v>69</v>
-      </c>
       <c r="K9">
         <v>2887</v>
       </c>
       <c r="L9" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="M9" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="N9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" t="s">
         <v>22</v>
@@ -1729,46 +1591,43 @@
       <c r="I10">
         <v>0.35</v>
       </c>
-      <c r="J10" t="s">
-        <v>75</v>
-      </c>
       <c r="K10">
         <v>6202</v>
       </c>
       <c r="L10" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="M10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="N10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" t="s">
         <v>22</v>
@@ -1779,46 +1638,43 @@
       <c r="I11">
         <v>3.1</v>
       </c>
-      <c r="J11" t="s">
-        <v>48</v>
-      </c>
       <c r="K11">
         <v>420</v>
       </c>
       <c r="L11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="M11" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="N11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" t="s">
         <v>22</v>
@@ -1829,46 +1685,43 @@
       <c r="I12">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J12" t="s">
-        <v>84</v>
-      </c>
       <c r="K12">
         <v>143020</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="M12" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="N12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G13" t="s">
         <v>22</v>
@@ -1879,46 +1732,43 @@
       <c r="I13">
         <v>0.12</v>
       </c>
-      <c r="J13" t="s">
-        <v>90</v>
-      </c>
       <c r="K13">
         <v>3290</v>
       </c>
       <c r="L13" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="M13" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="N13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O13" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" t="s">
         <v>27</v>
-      </c>
-      <c r="P13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G14" t="s">
         <v>22</v>
@@ -1929,46 +1779,43 @@
       <c r="I14">
         <v>0.71</v>
       </c>
-      <c r="J14" t="s">
-        <v>97</v>
-      </c>
       <c r="K14">
         <v>132362</v>
       </c>
       <c r="L14" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="M14" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="N14" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="O14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G15" t="s">
         <v>22</v>
@@ -1979,46 +1826,43 @@
       <c r="I15">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J15" t="s">
-        <v>105</v>
-      </c>
       <c r="K15">
         <v>5805</v>
       </c>
       <c r="L15" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="M15" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="N15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="E16" t="s">
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G16" t="s">
         <v>22</v>
@@ -2029,46 +1873,43 @@
       <c r="I16">
         <v>0.95</v>
       </c>
-      <c r="J16" t="s">
-        <v>111</v>
-      </c>
       <c r="K16">
         <v>24808</v>
       </c>
       <c r="L16" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M16" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="N16" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="O16" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16" t="s">
         <v>27</v>
-      </c>
-      <c r="P16" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D17" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
         <v>22</v>
@@ -2079,46 +1920,43 @@
       <c r="I17">
         <v>1.58</v>
       </c>
-      <c r="J17" t="s">
-        <v>117</v>
-      </c>
       <c r="K17">
         <v>11235</v>
       </c>
       <c r="L17" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M17" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="N17" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="O17" t="s">
+        <v>26</v>
+      </c>
+      <c r="P17" t="s">
         <v>27</v>
-      </c>
-      <c r="P17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="E18" t="s">
         <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G18" t="s">
         <v>22</v>
@@ -2129,46 +1967,43 @@
       <c r="I18">
         <v>2.52</v>
       </c>
-      <c r="J18" t="s">
-        <v>123</v>
-      </c>
       <c r="K18">
         <v>1656</v>
       </c>
       <c r="L18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M18" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="N18" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="O18" t="s">
+        <v>26</v>
+      </c>
+      <c r="P18" t="s">
         <v>27</v>
-      </c>
-      <c r="P18" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D19" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="E19" t="s">
         <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19" t="s">
         <v>22</v>
@@ -2179,46 +2014,43 @@
       <c r="I19">
         <v>0.4</v>
       </c>
-      <c r="J19" t="s">
-        <v>129</v>
-      </c>
       <c r="K19">
         <v>56700</v>
       </c>
       <c r="L19" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="M19" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="N19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="D20" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="E20" t="s">
         <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" t="s">
         <v>22</v>
@@ -2229,46 +2061,43 @@
       <c r="I20">
         <v>0.5</v>
       </c>
-      <c r="J20" t="s">
-        <v>135</v>
-      </c>
       <c r="K20">
         <v>19637</v>
       </c>
       <c r="L20" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M20" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="N20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B21" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="D21" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="E21" t="s">
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="G21" t="s">
         <v>22</v>
@@ -2279,46 +2108,43 @@
       <c r="I21">
         <v>3.58</v>
       </c>
-      <c r="J21" t="s">
-        <v>142</v>
-      </c>
       <c r="K21">
         <v>516</v>
       </c>
       <c r="L21" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="M21" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="N21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C22" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="D22" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="E22" t="s">
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="G22" t="s">
         <v>22</v>
@@ -2329,46 +2155,43 @@
       <c r="I22">
         <v>3.76</v>
       </c>
-      <c r="J22" t="s">
-        <v>147</v>
-      </c>
       <c r="K22">
         <v>908</v>
       </c>
       <c r="L22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="M22" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="N22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C23" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D23" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="E23" t="s">
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G23" t="s">
         <v>22</v>
@@ -2379,46 +2202,43 @@
       <c r="I23">
         <v>0.13</v>
       </c>
-      <c r="J23" t="s">
-        <v>152</v>
-      </c>
       <c r="K23">
         <v>155717</v>
       </c>
       <c r="L23" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="M23" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="N23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="B24" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="C24" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="E24" t="s">
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G24" t="s">
         <v>22</v>
@@ -2429,40 +2249,37 @@
       <c r="I24">
         <v>1.02</v>
       </c>
-      <c r="J24" t="s">
-        <v>159</v>
-      </c>
       <c r="K24">
         <v>2623</v>
       </c>
       <c r="L24" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="M24" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="N24" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="O24" t="s">
+        <v>26</v>
+      </c>
+      <c r="P24" t="s">
         <v>27</v>
-      </c>
-      <c r="P24" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="B25" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="C25" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="D25" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="E25" t="s">
         <v>20</v>
@@ -2479,46 +2296,43 @@
       <c r="I25">
         <v>13.59</v>
       </c>
-      <c r="J25" t="s">
-        <v>166</v>
-      </c>
       <c r="K25">
         <v>744</v>
       </c>
       <c r="L25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M25" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="N25" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="O25" t="s">
+        <v>26</v>
+      </c>
+      <c r="P25" t="s">
         <v>27</v>
-      </c>
-      <c r="P25" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="B26" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C26" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="D26" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="E26" t="s">
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G26" t="s">
         <v>22</v>
@@ -2529,46 +2343,43 @@
       <c r="I26">
         <v>0.66</v>
       </c>
-      <c r="J26" t="s">
-        <v>172</v>
-      </c>
       <c r="K26">
         <v>115972</v>
       </c>
       <c r="L26" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="M26" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="N26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="B27" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C27" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="D27" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="E27" t="s">
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G27" t="s">
         <v>22</v>
@@ -2579,46 +2390,43 @@
       <c r="I27">
         <v>0.66</v>
       </c>
-      <c r="J27" t="s">
-        <v>172</v>
-      </c>
       <c r="K27">
         <v>4031</v>
       </c>
       <c r="L27" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="M27" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="N27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B28" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="C28" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="D28" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="E28" t="s">
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G28" t="s">
         <v>22</v>
@@ -2629,46 +2437,43 @@
       <c r="I28">
         <v>1.65</v>
       </c>
-      <c r="J28" t="s">
-        <v>183</v>
-      </c>
       <c r="K28">
         <v>6570</v>
       </c>
       <c r="L28" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M28" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="N28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O28" t="s">
+        <v>26</v>
+      </c>
+      <c r="P28" t="s">
         <v>27</v>
-      </c>
-      <c r="P28" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="B29" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="C29" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="D29" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="E29" t="s">
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G29" t="s">
         <v>22</v>
@@ -2679,46 +2484,43 @@
       <c r="I29">
         <v>0.86</v>
       </c>
-      <c r="J29" t="s">
-        <v>189</v>
-      </c>
       <c r="K29">
         <v>2089</v>
       </c>
       <c r="L29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M29" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
       <c r="N29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O29" t="s">
+        <v>26</v>
+      </c>
+      <c r="P29" t="s">
         <v>27</v>
-      </c>
-      <c r="P29" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="B30" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="D30" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="E30" t="s">
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G30" t="s">
         <v>22</v>
@@ -2729,96 +2531,90 @@
       <c r="I30">
         <v>0.47</v>
       </c>
-      <c r="J30" t="s">
-        <v>195</v>
-      </c>
       <c r="K30">
         <v>169915</v>
       </c>
       <c r="L30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M30" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="N30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="B31" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="C31" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="D31" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="E31" t="s">
         <v>20</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G31" t="s">
         <v>22</v>
       </c>
       <c r="H31">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I31">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J31" t="s">
-        <v>200</v>
-      </c>
       <c r="K31">
         <v>320718</v>
       </c>
       <c r="L31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M31" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="N31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>202</v>
+        <v>174</v>
       </c>
       <c r="B32" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="C32" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="D32" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="E32" t="s">
         <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G32" t="s">
         <v>22</v>
@@ -2829,46 +2625,43 @@
       <c r="I32">
         <v>0.18</v>
       </c>
-      <c r="J32" t="s">
-        <v>205</v>
-      </c>
       <c r="K32">
         <v>63577</v>
       </c>
       <c r="L32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M32" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="N32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="B33" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="C33" t="s">
-        <v>208</v>
+        <v>179</v>
       </c>
       <c r="D33" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="E33" t="s">
         <v>20</v>
       </c>
       <c r="F33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G33" t="s">
         <v>22</v>
@@ -2879,46 +2672,43 @@
       <c r="I33">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="J33" t="s">
-        <v>210</v>
-      </c>
       <c r="K33">
         <v>1575456</v>
       </c>
       <c r="L33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M33" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="N33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="B34" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="D34" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="E34" t="s">
         <v>20</v>
       </c>
       <c r="F34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G34" t="s">
         <v>22</v>
@@ -2929,46 +2719,43 @@
       <c r="I34">
         <v>0.2</v>
       </c>
-      <c r="J34" t="s">
-        <v>129</v>
-      </c>
       <c r="K34">
         <v>55985</v>
       </c>
       <c r="L34" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M34" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="N34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="B35" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="C35" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="D35" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
       <c r="E35" t="s">
         <v>20</v>
       </c>
       <c r="F35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G35" t="s">
         <v>22</v>
@@ -2979,46 +2766,43 @@
       <c r="I35">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="J35" t="s">
-        <v>218</v>
-      </c>
       <c r="K35">
         <v>1804980</v>
       </c>
       <c r="L35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M35" t="s">
-        <v>219</v>
+        <v>188</v>
       </c>
       <c r="N35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="B36" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="C36" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="D36" t="s">
-        <v>223</v>
+        <v>192</v>
       </c>
       <c r="E36" t="s">
         <v>20</v>
       </c>
       <c r="F36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G36" t="s">
         <v>22</v>
@@ -3029,46 +2813,43 @@
       <c r="I36">
         <v>0.35</v>
       </c>
-      <c r="J36" t="s">
-        <v>224</v>
-      </c>
       <c r="K36">
         <v>15088</v>
       </c>
       <c r="L36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M36" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="N36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O36" t="s">
+        <v>26</v>
+      </c>
+      <c r="P36" t="s">
         <v>27</v>
-      </c>
-      <c r="P36" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="B37" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="C37" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="D37" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="E37" t="s">
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G37" t="s">
         <v>22</v>
@@ -3079,46 +2860,43 @@
       <c r="I37">
         <v>0.35</v>
       </c>
-      <c r="J37" t="s">
-        <v>229</v>
-      </c>
       <c r="K37">
         <v>7514</v>
       </c>
       <c r="L37" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M37" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="N37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O37" t="s">
+        <v>26</v>
+      </c>
+      <c r="P37" t="s">
         <v>27</v>
-      </c>
-      <c r="P37" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>230</v>
+        <v>197</v>
       </c>
       <c r="B38" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="C38" t="s">
-        <v>231</v>
+        <v>198</v>
       </c>
       <c r="D38" t="s">
-        <v>232</v>
+        <v>199</v>
       </c>
       <c r="E38" t="s">
         <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G38" t="s">
         <v>22</v>
@@ -3129,46 +2907,43 @@
       <c r="I38">
         <v>0.35</v>
       </c>
-      <c r="J38" t="s">
-        <v>75</v>
-      </c>
       <c r="K38">
         <v>7655</v>
       </c>
       <c r="L38" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M38" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="N38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O38" t="s">
+        <v>26</v>
+      </c>
+      <c r="P38" t="s">
         <v>27</v>
-      </c>
-      <c r="P38" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>233</v>
+        <v>200</v>
       </c>
       <c r="B39" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s">
-        <v>234</v>
+        <v>201</v>
       </c>
       <c r="D39" t="s">
-        <v>235</v>
+        <v>202</v>
       </c>
       <c r="E39" t="s">
         <v>20</v>
       </c>
       <c r="F39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G39" t="s">
         <v>22</v>
@@ -3179,46 +2954,43 @@
       <c r="I39">
         <v>0.1</v>
       </c>
-      <c r="J39" t="s">
-        <v>236</v>
-      </c>
       <c r="K39">
         <v>489828</v>
       </c>
       <c r="L39" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M39" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="N39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="B40" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C40" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
       <c r="D40" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
       <c r="E40" t="s">
         <v>20</v>
       </c>
       <c r="F40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G40" t="s">
         <v>22</v>
@@ -3229,46 +3001,43 @@
       <c r="I40">
         <v>0.1</v>
       </c>
-      <c r="J40" t="s">
-        <v>241</v>
-      </c>
       <c r="K40">
         <v>65782</v>
       </c>
       <c r="L40" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M40" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="N40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="B41" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C41" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="D41" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="E41" t="s">
         <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G41" t="s">
         <v>22</v>
@@ -3279,46 +3048,43 @@
       <c r="I41">
         <v>0.1</v>
       </c>
-      <c r="J41" t="s">
-        <v>129</v>
-      </c>
       <c r="K41">
         <v>177541</v>
       </c>
       <c r="L41" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M41" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="N41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P41" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="B42" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C42" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="D42" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="E42" t="s">
         <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G42" t="s">
         <v>22</v>
@@ -3329,46 +3095,43 @@
       <c r="I42">
         <v>0.1</v>
       </c>
-      <c r="J42" t="s">
-        <v>250</v>
-      </c>
       <c r="K42">
         <v>298436</v>
       </c>
       <c r="L42" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M42" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
       <c r="N42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P42" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
       <c r="B43" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C43" t="s">
-        <v>253</v>
+        <v>217</v>
       </c>
       <c r="D43" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G43" t="s">
         <v>22</v>
@@ -3379,46 +3142,43 @@
       <c r="I43">
         <v>0.1</v>
       </c>
-      <c r="J43" t="s">
-        <v>250</v>
-      </c>
       <c r="K43">
         <v>118618</v>
       </c>
       <c r="L43" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M43" t="s">
-        <v>255</v>
+        <v>219</v>
       </c>
       <c r="N43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P43" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>256</v>
+        <v>220</v>
       </c>
       <c r="B44" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C44" t="s">
-        <v>257</v>
+        <v>221</v>
       </c>
       <c r="D44" t="s">
-        <v>258</v>
+        <v>222</v>
       </c>
       <c r="E44" t="s">
         <v>20</v>
       </c>
       <c r="F44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G44" t="s">
         <v>22</v>
@@ -3429,46 +3189,43 @@
       <c r="I44">
         <v>0.1</v>
       </c>
-      <c r="J44" t="s">
-        <v>259</v>
-      </c>
       <c r="K44">
         <v>606430</v>
       </c>
       <c r="L44" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M44" t="s">
-        <v>260</v>
+        <v>223</v>
       </c>
       <c r="N44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P44" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>261</v>
+        <v>224</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C45" t="s">
-        <v>262</v>
+        <v>225</v>
       </c>
       <c r="D45" t="s">
-        <v>282</v>
+        <v>244</v>
       </c>
       <c r="E45" t="s">
         <v>20</v>
       </c>
       <c r="F45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G45" t="s">
         <v>22</v>
@@ -3479,46 +3236,43 @@
       <c r="I45">
         <v>0.1</v>
       </c>
-      <c r="J45" t="s">
-        <v>241</v>
-      </c>
       <c r="K45">
         <v>746294</v>
       </c>
       <c r="L45" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M45" t="s">
-        <v>263</v>
+        <v>226</v>
       </c>
       <c r="N45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P45" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>264</v>
+        <v>227</v>
       </c>
       <c r="B46" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C46" t="s">
-        <v>265</v>
+        <v>228</v>
       </c>
       <c r="D46" t="s">
-        <v>266</v>
+        <v>229</v>
       </c>
       <c r="E46" t="s">
         <v>20</v>
       </c>
       <c r="F46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G46" t="s">
         <v>22</v>
@@ -3529,46 +3283,43 @@
       <c r="I46">
         <v>0.1</v>
       </c>
-      <c r="J46" t="s">
-        <v>259</v>
-      </c>
       <c r="K46">
         <v>12317582</v>
       </c>
       <c r="L46" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M46" t="s">
-        <v>267</v>
+        <v>230</v>
       </c>
       <c r="N46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P46" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>268</v>
+        <v>231</v>
       </c>
       <c r="B47" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C47" t="s">
-        <v>269</v>
+        <v>232</v>
       </c>
       <c r="D47" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="E47" t="s">
         <v>20</v>
       </c>
       <c r="F47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G47" t="s">
         <v>22</v>
@@ -3579,46 +3330,43 @@
       <c r="I47">
         <v>0.1</v>
       </c>
-      <c r="J47" t="s">
-        <v>241</v>
-      </c>
       <c r="K47">
         <v>120542</v>
       </c>
       <c r="L47" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M47" t="s">
-        <v>271</v>
+        <v>234</v>
       </c>
       <c r="N47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>272</v>
+        <v>235</v>
       </c>
       <c r="B48" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="C48" t="s">
-        <v>273</v>
+        <v>236</v>
       </c>
       <c r="D48" t="s">
-        <v>281</v>
+        <v>243</v>
       </c>
       <c r="E48" t="s">
         <v>20</v>
       </c>
       <c r="F48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G48" t="s">
         <v>22</v>
@@ -3629,46 +3377,43 @@
       <c r="I48">
         <v>4.7E-2</v>
       </c>
-      <c r="J48" t="s">
-        <v>64</v>
-      </c>
       <c r="K48">
         <v>3123703</v>
       </c>
       <c r="L48" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M48" t="s">
-        <v>274</v>
+        <v>237</v>
       </c>
       <c r="N48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P48" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>275</v>
+        <v>238</v>
       </c>
       <c r="B49" t="s">
-        <v>276</v>
+        <v>239</v>
       </c>
       <c r="C49" t="s">
-        <v>277</v>
+        <v>240</v>
       </c>
       <c r="D49" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="E49" t="s">
         <v>20</v>
       </c>
       <c r="F49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G49" t="s">
         <v>22</v>
@@ -3679,26 +3424,23 @@
       <c r="I49">
         <v>0.7</v>
       </c>
-      <c r="J49" t="s">
-        <v>279</v>
-      </c>
       <c r="K49">
         <v>24887</v>
       </c>
       <c r="L49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M49" t="s">
-        <v>280</v>
+        <v>242</v>
       </c>
       <c r="N49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O49" t="s">
+        <v>26</v>
+      </c>
+      <c r="P49" t="s">
         <v>27</v>
-      </c>
-      <c r="P49" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>